<commit_message>
excel to objectarray, about us section
</commit_message>
<xml_diff>
--- a/OpenEmrApplication/TestData/OpenEMRData.xlsx
+++ b/OpenEmrApplication/TestData/OpenEMRData.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-Mine\Company\Company\Sollers\OpenEmrApplication\OpenEmrApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="AddPatientTest" sheetId="2" r:id="rId2"/>
+    <sheet name="AboutUsHeaderAndVersionTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Username</t>
   </si>
@@ -57,6 +59,81 @@
   </si>
   <si>
     <t>Rich</t>
+  </si>
+  <si>
+    <t>bal</t>
+  </si>
+  <si>
+    <t>bal123</t>
+  </si>
+  <si>
+    <t>Invalid username or password123</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ExpectedAlertText</t>
+  </si>
+  <si>
+    <t>ExpectedPatientName</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>English (Indian)</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>2021-07-19</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Assessment: Tobacco</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - John Ken</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - Bala Dina</t>
+  </si>
+  <si>
+    <t>ExpectedHeader</t>
+  </si>
+  <si>
+    <t>ExpectedVersion</t>
+  </si>
+  <si>
+    <t>About OpenEMR</t>
+  </si>
+  <si>
+    <t>Version Number: v6.0.0 (1)</t>
+  </si>
+  <si>
+    <t>physician</t>
   </si>
 </sst>
 </file>
@@ -92,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +508,202 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>